<commit_message>
Add reference volume data
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/hyperarc.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/hyperarc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="164">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -442,9 +442,6 @@
     <t>GTVs</t>
   </si>
   <si>
-    <t>GTVs_HD</t>
-  </si>
-  <si>
     <t>NerfOptDt+2</t>
   </si>
   <si>
@@ -515,6 +512,9 @@
   </si>
   <si>
     <t>hyperarc</t>
+  </si>
+  <si>
+    <t>GTVsHD</t>
   </si>
 </sst>
 </file>
@@ -1520,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -2579,8 +2579,8 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,9 +2634,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="12" t="s">
-        <v>90</v>
-      </c>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2683,7 +2681,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -2696,7 +2694,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2711,7 +2709,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2726,7 +2724,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2737,7 +2735,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2750,7 +2748,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -2763,7 +2761,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2774,20 +2772,18 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="12" t="s">
-        <v>90</v>
-      </c>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2810,8 +2806,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2845,7 +2841,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2" s="6">
         <v>400</v>
@@ -2860,7 +2856,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2871,7 +2867,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" s="6">
         <v>-400</v>
@@ -2951,7 +2947,7 @@
         <v>122</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2961,7 +2957,7 @@
         <v>123</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -2971,13 +2967,13 @@
         <v>119</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2985,7 +2981,7 @@
         <v>121</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2995,7 +2991,7 @@
         <v>129</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -3005,35 +3001,35 @@
         <v>130</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>